<commit_message>
cost calculation Excel model
</commit_message>
<xml_diff>
--- a/CSS_BOM_Parts_Catalogue.xlsx
+++ b/CSS_BOM_Parts_Catalogue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunet-my.sharepoint.com/personal/wshi2_lunet_lboro_ac_uk/Documents/hsuv_mms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wshi2\Desktop\hsuv_mms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_38A52DAE43429AAC924660E9FB8A75EF65BCDF72" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF007AF2-9468-4F83-A0C3-F29A89E2409F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25894D5A-B87B-4381-B8BF-829689ED5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="1500" windowWidth="17070" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18060" yWindow="1140" windowWidth="14400" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>